<commit_message>
change kpis and add tests
</commit_message>
<xml_diff>
--- a/Projects/PEPSICOUK/Tests/Data/Inclusion_Exclusion_Template.xlsx
+++ b/Projects/PEPSICOUK/Tests/Data/Inclusion_Exclusion_Template.xlsx
@@ -259,14 +259,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>